<commit_message>
Updating project management docs, adding backgrounds in the game.
</commit_message>
<xml_diff>
--- a/gestionProjet/Liste de Tâches.xlsx
+++ b/gestionProjet/Liste de Tâches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <r>
       <rPr>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Réalisation du dossier de projet</t>
+  </si>
+  <si>
+    <t>En cours de réalisation</t>
   </si>
 </sst>
 </file>
@@ -313,10 +316,10 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -345,6 +348,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -357,23 +377,6 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -715,16 +718,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:H18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Liste_de_tâches" displayName="Liste_de_tâches" ref="B4:H18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B4:H18"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Tâche" dataDxfId="7"/>
-    <tableColumn id="4" name="État " dataDxfId="6"/>
-    <tableColumn id="6" name="Date de début " dataDxfId="5"/>
-    <tableColumn id="7" name="Échéance " dataDxfId="4"/>
+    <tableColumn id="1" name="Tâche" dataDxfId="6"/>
+    <tableColumn id="4" name="État " dataDxfId="5"/>
+    <tableColumn id="6" name="Date de début " dataDxfId="4"/>
+    <tableColumn id="7" name="Échéance " dataDxfId="3"/>
     <tableColumn id="2" name="Date de Fin" dataDxfId="2"/>
-    <tableColumn id="5" name="% achevé" dataDxfId="0" dataCellStyle="Pourcentage"/>
-    <tableColumn id="9" name="Terminée/En retard ?" dataDxfId="1"/>
+    <tableColumn id="5" name="% achevé" dataDxfId="1" dataCellStyle="Pourcentage"/>
+    <tableColumn id="9" name="Terminée/En retard ?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -979,7 +982,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1077,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
         <v>42128</v>
@@ -1082,16 +1085,22 @@
       <c r="E7" s="7">
         <v>42130</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="7">
+        <v>42130</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>12</v>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D8" s="10">
         <v>42128</v>
@@ -1099,16 +1108,22 @@
       <c r="E8" s="10">
         <v>42134</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="10">
+        <v>42134</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>12</v>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D9" s="10">
         <v>42131</v>
@@ -1116,16 +1131,22 @@
       <c r="E9" s="10">
         <v>42134</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="5"/>
+      <c r="F9" s="10">
+        <v>42134</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>12</v>
+      <c r="C10" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D10" s="10">
         <v>42135</v>
@@ -1133,16 +1154,22 @@
       <c r="E10" s="10">
         <v>42137</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="5"/>
+      <c r="F10" s="10">
+        <v>42137</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>12</v>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D11" s="10">
         <v>42135</v>
@@ -1150,16 +1177,22 @@
       <c r="E11" s="10">
         <v>42137</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="5"/>
+      <c r="F11" s="10">
+        <v>42137</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>12</v>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D12" s="10">
         <v>42138</v>
@@ -1167,16 +1200,22 @@
       <c r="E12" s="10">
         <v>42141</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="5"/>
+      <c r="F12" s="10">
+        <v>42141</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>12</v>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D13" s="10">
         <v>42138</v>
@@ -1184,16 +1223,22 @@
       <c r="E13" s="10">
         <v>42141</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="5"/>
+      <c r="F13" s="10">
+        <v>42141</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D14" s="10">
         <v>42142</v>

</xml_diff>